<commit_message>
v1.1 update owner status after modify ERD
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_ERD_REVIEW.xlsx
+++ b/LH_REVIEWS/LH_ERD_REVIEW.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC77055D-D2C8-4603-9FE4-1478C9CDABF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
+    <sheet name="LH_ERD_REVIEW" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -146,12 +145,27 @@
   </si>
   <si>
     <t>30/4/2025</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>v11</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>update owner status after modify ERD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -341,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -440,9 +454,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -724,11 +735,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,7 +786,7 @@
     </row>
     <row r="2" spans="1:9" ht="45">
       <c r="A2" s="5">
-        <f>DATE(2025,4,30)</f>
+        <f t="shared" ref="A2:A8" si="0">DATE(2025,4,30)</f>
         <v>45777</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -797,7 +808,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>27</v>
@@ -805,7 +816,7 @@
     </row>
     <row r="3" spans="1:9" ht="47.25" customHeight="1">
       <c r="A3" s="6">
-        <f>DATE(2025,4,30)</f>
+        <f t="shared" si="0"/>
         <v>45777</v>
       </c>
       <c r="B3" s="25" t="s">
@@ -827,7 +838,7 @@
         <v>26</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>27</v>
@@ -835,7 +846,7 @@
     </row>
     <row r="4" spans="1:9" ht="30">
       <c r="A4" s="5">
-        <f>DATE(2025,4,30)</f>
+        <f t="shared" si="0"/>
         <v>45777</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -857,7 +868,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>27</v>
@@ -865,7 +876,7 @@
     </row>
     <row r="5" spans="1:9" ht="33" customHeight="1">
       <c r="A5" s="6">
-        <f>DATE(2025,4,30)</f>
+        <f t="shared" si="0"/>
         <v>45777</v>
       </c>
       <c r="B5" s="28" t="s">
@@ -887,7 +898,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I5" s="30" t="s">
         <v>27</v>
@@ -895,7 +906,7 @@
     </row>
     <row r="6" spans="1:9" ht="34.5" customHeight="1">
       <c r="A6" s="5">
-        <f>DATE(2025,4,30)</f>
+        <f t="shared" si="0"/>
         <v>45777</v>
       </c>
       <c r="B6" s="22" t="s">
@@ -917,7 +928,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>27</v>
@@ -925,7 +936,7 @@
     </row>
     <row r="7" spans="1:9" ht="30">
       <c r="A7" s="6">
-        <f>DATE(2025,4,30)</f>
+        <f t="shared" si="0"/>
         <v>45777</v>
       </c>
       <c r="B7" s="28" t="s">
@@ -947,7 +958,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I7" s="30" t="s">
         <v>27</v>
@@ -955,7 +966,7 @@
     </row>
     <row r="8" spans="1:9" ht="33" customHeight="1">
       <c r="A8" s="5">
-        <f>DATE(2025,4,30)</f>
+        <f t="shared" si="0"/>
         <v>45777</v>
       </c>
       <c r="B8" s="22" t="s">
@@ -1034,10 +1045,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1046,11 +1057,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1089,11 +1100,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="34"/>
+    <row r="3" spans="1:4" ht="37.5">
+      <c r="A3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="33">
+        <v>45662</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="10"/>

</xml_diff>